<commit_message>
Clean Code and Codebook
</commit_message>
<xml_diff>
--- a/4_Data_Extraction/4_2_Open_Data/Paper_6/CodeBook_Data_for_p6_Exp1.xlsx
+++ b/4_Data_Extraction/4_2_Open_Data/Paper_6/CodeBook_Data_for_p6_Exp1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
   <si>
     <t>Variable_name</t>
   </si>
@@ -47,97 +47,100 @@
     <t>Shape assigned to each participant</t>
   </si>
   <si>
+    <t>P1,P2,Stranger</t>
+  </si>
+  <si>
+    <t>Categorical</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Label associated with the shape</t>
+  </si>
+  <si>
+    <t>ShapeLoc</t>
+  </si>
+  <si>
+    <t>Location of the shape in the experiment</t>
+  </si>
+  <si>
+    <t>Top,Bottom</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Judging whether specific shapes and labels match or mismatch</t>
+  </si>
+  <si>
+    <t>Match,Mismatch</t>
+  </si>
+  <si>
+    <t>.thisRepN</t>
+  </si>
+  <si>
+    <t>Repetition number in the current trial</t>
+  </si>
+  <si>
+    <t>Numeric</t>
+  </si>
+  <si>
+    <t>Continuous</t>
+  </si>
+  <si>
+    <t>.thisTrialN</t>
+  </si>
+  <si>
+    <t>Trial number in the current session</t>
+  </si>
+  <si>
+    <t>.thisN</t>
+  </si>
+  <si>
+    <t>Total number of trials in the current session</t>
+  </si>
+  <si>
+    <t>.thisIndex</t>
+  </si>
+  <si>
+    <t>Index of the current trial</t>
+  </si>
+  <si>
+    <t>resp</t>
+  </si>
+  <si>
+    <t>Participant's response to the stimulus</t>
+  </si>
+  <si>
+    <t>o,w,None</t>
+  </si>
+  <si>
+    <t>rt</t>
+  </si>
+  <si>
+    <t>Response time in milliseconds</t>
+  </si>
+  <si>
+    <t>Exclude</t>
+  </si>
+  <si>
+    <t>Exclusion indicator for data analysis</t>
+  </si>
+  <si>
+    <t>0, 1</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>StrangerShape</t>
+  </si>
+  <si>
+    <t>Shape assigned to the stranger</t>
+  </si>
+  <si>
     <t>Triangle, Diamond, Circle, Pentagon, Star</t>
-  </si>
-  <si>
-    <t>Categorical</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>Label associated with the shape</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>ShapeLoc</t>
-  </si>
-  <si>
-    <t>Location of the shape in the experiment</t>
-  </si>
-  <si>
-    <t>Above, Below</t>
-  </si>
-  <si>
-    <t>Condition</t>
-  </si>
-  <si>
-    <t>Different conditions or contexts in the experiment</t>
-  </si>
-  <si>
-    <t>Self, Partner, Stranger</t>
-  </si>
-  <si>
-    <t>.thisRepN</t>
-  </si>
-  <si>
-    <t>Repetition number in the current trial</t>
-  </si>
-  <si>
-    <t>Numeric</t>
-  </si>
-  <si>
-    <t>Continuous</t>
-  </si>
-  <si>
-    <t>.thisTrialN</t>
-  </si>
-  <si>
-    <t>Trial number in the current session</t>
-  </si>
-  <si>
-    <t>.thisN</t>
-  </si>
-  <si>
-    <t>Total number of trials in the current session</t>
-  </si>
-  <si>
-    <t>.thisIndex</t>
-  </si>
-  <si>
-    <t>Index of the current trial</t>
-  </si>
-  <si>
-    <t>resp</t>
-  </si>
-  <si>
-    <t>Participant's response to the stimulus</t>
-  </si>
-  <si>
-    <t>rt</t>
-  </si>
-  <si>
-    <t>Response time in milliseconds</t>
-  </si>
-  <si>
-    <t>Exclude</t>
-  </si>
-  <si>
-    <t>Exclusion indicator for data analysis</t>
-  </si>
-  <si>
-    <t>0, 1</t>
-  </si>
-  <si>
-    <t>Binary</t>
-  </si>
-  <si>
-    <t>StrangerShape</t>
-  </si>
-  <si>
-    <t>Shape assigned to the stranger</t>
   </si>
   <si>
     <t>P1Shape</t>
@@ -1368,13 +1371,13 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="19.6363636363636" customWidth="1"/>
-    <col min="2" max="2" width="56.8181818181818" customWidth="1"/>
+    <col min="2" max="2" width="68" customWidth="1"/>
     <col min="3" max="3" width="46.6363636363636" customWidth="1"/>
     <col min="4" max="4" width="19.6363636363636" customWidth="1"/>
   </cols>
@@ -1415,7 +1418,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -1423,13 +1426,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -1437,13 +1440,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -1451,69 +1454,69 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
       <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
         <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
       <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
         <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
       <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -1527,10 +1530,10 @@
         <v>30</v>
       </c>
       <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
         <v>19</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1555,7 +1558,7 @@
         <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -1563,13 +1566,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
         <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
@@ -1577,13 +1580,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -1591,10 +1594,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
         <v>33</v>
@@ -1605,10 +1608,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
         <v>33</v>
@@ -1619,69 +1622,69 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
         <v>19</v>
-      </c>
-      <c r="D18" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
         <v>19</v>
-      </c>
-      <c r="D19" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
         <v>19</v>
-      </c>
-      <c r="D20" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
         <v>19</v>
-      </c>
-      <c r="D21" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
@@ -1689,41 +1692,41 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
         <v>19</v>
-      </c>
-      <c r="D23" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" t="s">
         <v>19</v>
-      </c>
-      <c r="D24" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>

</xml_diff>